<commit_message>
Create working extraction of trial balance, income statement, balance sheet
</commit_message>
<xml_diff>
--- a/data/Manufacturing_Accounting_Simple.xlsx
+++ b/data/Manufacturing_Accounting_Simple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\chai\chaihub\finance-tools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C044DBA-7F61-4203-9DC5-DDA9B65BCCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84A4F38-0C54-4562-9126-8D76319A2C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart_of_Accounts" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,13 +193,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -214,8 +228,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,7 +536,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -529,134 +547,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1000</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>1100</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>1200</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>1500</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>2000</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>3000</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>3100</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>4000</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>5000</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>5100</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>5200</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -669,7 +687,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -680,222 +700,214 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1000</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>2000000</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>3000</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>0</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>2000000</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>1200</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>500000</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1">
+        <v>500000</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1100</v>
+      </c>
+      <c r="D6" s="1">
+        <v>800000</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4000</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <v>800000</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5000</v>
+      </c>
+      <c r="D8" s="1">
+        <v>350000</v>
+      </c>
+      <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5">
-        <v>2000</v>
-      </c>
-      <c r="D5">
+      <c r="F8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1200</v>
+      </c>
+      <c r="D9" s="1">
         <v>0</v>
       </c>
-      <c r="E5">
-        <v>500000</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6">
-        <v>1100</v>
-      </c>
-      <c r="D6">
-        <v>800000</v>
-      </c>
-      <c r="E6">
+      <c r="E9" s="1">
+        <v>350000</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5100</v>
+      </c>
+      <c r="D10" s="1">
+        <v>150000</v>
+      </c>
+      <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7">
-        <v>4000</v>
-      </c>
-      <c r="D7">
+      <c r="F10" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D11" s="1">
         <v>0</v>
       </c>
-      <c r="E7">
-        <v>800000</v>
-      </c>
-      <c r="F7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8">
-        <v>5000</v>
-      </c>
-      <c r="D8">
-        <v>350000</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9">
-        <v>1200</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>350000</v>
-      </c>
-      <c r="F9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10">
-        <v>5100</v>
-      </c>
-      <c r="D10">
+      <c r="E11" s="1">
         <v>150000</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11">
-        <v>1000</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>150000</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -908,7 +920,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -917,16 +931,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -939,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -949,56 +963,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2">
-        <f>800000</f>
-        <v>800000</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3">
-        <f>350000</f>
-        <v>350000</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4">
-        <f>B2-B3</f>
-        <v>450000</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5">
-        <f>150000</f>
-        <v>150000</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B6">
-        <f>B4-B5</f>
-        <v>300000</v>
       </c>
     </row>
   </sheetData>
@@ -1010,7 +1004,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1019,65 +1015,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <f>2000000-150000</f>
-        <v>1850000</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
-        <f>2000000</f>
-        <v>2000000</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <f>150000</f>
-        <v>150000</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3">
-        <f>500000</f>
-        <v>500000</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <f>800000</f>
-        <v>800000</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D4">
-        <f>B5</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>